<commit_message>
agrego cambios casos de prueba
agrego documento
</commit_message>
<xml_diff>
--- a/evidenciaCaosPrueba.xlsx
+++ b/evidenciaCaosPrueba.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>Estado</t>
   </si>
@@ -58,16 +58,6 @@
   </si>
   <si>
     <t>CPHU01-07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dirigirse a la dirección
-http://localhost:4200/registro-usuario
-Dilgenciar los siguientes campos con la siguiente información
-Documento Identidad = 1023456783
-Nombre = Arturo Enrique
-Primer apellido = M
-Fecha de Nacimiento = 14/05/1997
-</t>
   </si>
   <si>
     <t>Dirigirse a la dirección
@@ -79,6 +69,156 @@
 Segundo apellido = Díaz
 Fecha de Nacimiento = 14/03/1993
 Seleccionar el boton Guardar Datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dirigirse a la dirección
+http://localhost:4200/registro-usuario
+Dilgenciar los siguientes campos con la siguiente información
+Documento Identidad = 1023456783
+Nombre = Arturo Enrique
+Primer apellido = M
+Fecha de Nacimiento = 14/05/1997
+Seleccionar el boton Guardar Datos
+</t>
+  </si>
+  <si>
+    <t>Dirigirse a la dirección
+http://localhost:4200/registro-usuario
+Dilgenciar los siguientes campos con la siguiente información
+Documento Identidad = 1076543894
+Nombre = Lui5
+ Apellido = Martínez
+Fecha de Nacimiento = 14/03/1993
+Seleccionar el boton Guardar Datos</t>
+  </si>
+  <si>
+    <t>Dirigirse a la dirección
+http://localhost:4200/registro-usuario
+Dilgenciar los siguientes campos con la siguiente información
+Documento Identidad = 123
+Nombre = Luis
+Apellido = Calle
+Fecha de Nacimiento = 14/03/1993
+Seleccionar el boton Guardar Datos</t>
+  </si>
+  <si>
+    <t>Dirigirse a la dirección
+http://localhost:4200/registro-usuario
+Dilgenciar los siguientes campos con la siguiente información
+Documento Identidad = 1089706320
+- Nombre = Manuel
+- Apellido = Díaz
+- Fecha de Nacimiento = 23 de diciembre del 83
+Seleccionar el boton Guardar Datos</t>
+  </si>
+  <si>
+    <t>Dirigirse a la dirección
+http://localhost:4200/registro-usuario
+Dilgenciar los siguientes campos con la siguiente información
+Documento Identidad = 1089706320
+- Nombre = Cristian
+- Apellido = Montoya
+- Fecha de Nacimiento = 14/11/2005
+Seleccionar el boton Guardar Datos</t>
+  </si>
+  <si>
+    <t>Dirigirse a la dirección
+http://localhost:4200/registro-usuario
+Dilgenciar los siguientes campos con la siguiente información
+Documento Identidad = 
+Nombre = Carlos
+- Apellido = Duarte
+- Fecha de Nacimiento = 30/10/1990
+Seleccionar el boton Guardar Datos</t>
+  </si>
+  <si>
+    <t>HU02</t>
+  </si>
+  <si>
+    <t>CPHU2-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seguir el caso de prueba CPHU01-01 diligenciando un documento de identidad aleatorio que no este ya registrado en la base de datos
+Diligenciar los siguientes campos con la siguiente información
+Nombre de Empresa = Accenture
+Tipo Nit = Jurídica 
+Nit = 800110980-7
+Salario Actual = 950000
+Fecha de Ingreso = 22/02/2018
+Seleccionar el boton Generar.
+</t>
+  </si>
+  <si>
+    <t>CPHU2-02</t>
+  </si>
+  <si>
+    <t>CPHU2-03</t>
+  </si>
+  <si>
+    <t>CPHU2-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depentiente del 
+caso de rueba </t>
+  </si>
+  <si>
+    <t>Seguir el caso de prueba CPHU01-01 diligenciando un documento de identidad aleatorio que no este ya registrado en la base de datos
+Diligenciar los siguientes campos con la siguiente información
+Nombre de Empresa = Empresa1
+Tipo Nit = Natural 
+Nit = 8736534234
+Salario Actual = tres millones
+Fecha de Ingreso = 01/02/2005
+Seleccionar el boton Generar.</t>
+  </si>
+  <si>
+    <t>Seguir el caso de prueba CPHU01-01 diligenciando un documento de identidad aleatorio que no este ya registrado en la base de datos
+Diligenciar los siguientes campos con la siguiente información
+Nombre de Empresa = E
+Tipo Nit = Jurídica 
+Nit = 800670890-1
+Salario Actual = 2500000
+Fecha de Ingreso = 01/02/2017
+Seleccionar el boton Generar.</t>
+  </si>
+  <si>
+    <t>Seguir el caso de prueba CPHU01-01 diligenciando un documento de identidad aleatorio que no este ya registrado en la base de datos
+Diligenciar los siguientes campos con la siguiente información
+Nombre de Empresa = Emoresa3
+Tipo Nit = Natural 
+Nit = 8006708976
+Salario Actual = 1000000
+Fecha de Ingreso = 1 de enero del 2017
+Seleccionar el boton Generar.</t>
+  </si>
+  <si>
+    <t>CPHU2-05</t>
+  </si>
+  <si>
+    <t>Seguir el caso de prueba CPHU01-01 diligenciando un documento de identidad aleatorio que no este ya registrado en la base de datos
+Diligenciar los siguientes campos con la siguiente información
+Nombre de Empresa = Emoresa5
+Tipo Nit = Jurídica 
+Nit = 500670890-1
+Salario Actual = 8000000
+Fecha de Ingreso = 01/12/2017
+Seleccionar el boton Generar.</t>
+  </si>
+  <si>
+    <t>CPHU2-06</t>
+  </si>
+  <si>
+    <t>Seguir el caso de prueba CPHU01-01 diligenciando un documento de identidad aleatorio que no este ya registrado en la base de datos
+Diligenciar los siguientes campos con la siguiente información
+Nombre de Empresa = Emoresa8
+Tipo Nit = Natural
+Nit = 6007809102
+Salario Actual = 
+Fecha de Ingreso = 11/12/1999
+Seleccionar el boton Generar.</t>
+  </si>
+  <si>
+    <t>N.A</t>
   </si>
 </sst>
 </file>
@@ -114,13 +254,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -405,83 +542,225 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="183" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>